<commit_message>
cards, data labels, start of img download
</commit_message>
<xml_diff>
--- a/data/source/house_price_index.xlsx
+++ b/data/source/house_price_index.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\SEM Update 2019\Data Sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\aboddupalli\Box Sync\TPC\CENTER\SLFI\Interactive Data Tools\SEM\SEM Update 2019\Data Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_1" sheetId="2" r:id="rId1"/>
@@ -2711,9 +2711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA212"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -26270,9 +26270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>